<commit_message>
Solved test connection bug. However, there is a known java bug which leads to trying several times a connection if the credentials are wrong. This leads to the block of the user DCF account. How to solve?
</commit_message>
<xml_diff>
--- a/doc/errors/errors.xlsx
+++ b/doc/errors/errors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20010" windowHeight="6240" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20010" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Error codes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="139">
   <si>
     <t>Error</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t>Username which does not exist/ wrong password / not authorized</t>
+  </si>
+  <si>
+    <t>The downloaded dataset contains data which do not follow the formulas defined in the excel. This can be due to old versions of datasets that were created with different formulas.</t>
+  </si>
+  <si>
+    <t>General runtime error, see message error stack for more information</t>
+  </si>
+  <si>
+    <t>XERRX</t>
   </si>
 </sst>
 </file>
@@ -840,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,6 +937,17 @@
         <v>91</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
@@ -1046,6 +1066,17 @@
         <v>49</v>
       </c>
       <c r="C21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1499,7 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added report validator and html table to see report errors
</commit_message>
<xml_diff>
--- a/doc/errors/errors.xlsx
+++ b/doc/errors/errors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="145">
   <si>
     <t>Error</t>
   </si>
@@ -433,6 +433,24 @@
   </si>
   <si>
     <t>XERRX</t>
+  </si>
+  <si>
+    <t>Axx</t>
+  </si>
+  <si>
+    <t>input/output errors</t>
+  </si>
+  <si>
+    <t>The file cannot be written into the selected folder. Either it does not exist or it is blocked by another program.</t>
+  </si>
+  <si>
+    <t>ERRA00</t>
+  </si>
+  <si>
+    <t>WARN001</t>
+  </si>
+  <si>
+    <t>The 'check report' validation of a report is not passed (validation fired from the check report in the toolbar)</t>
   </si>
 </sst>
 </file>
@@ -524,8 +542,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C57" totalsRowShown="0">
-  <autoFilter ref="A1:C57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C60" totalsRowShown="0">
+  <autoFilter ref="A1:C60"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Error"/>
     <tableColumn id="2" name="Error code"/>
@@ -536,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Error code group"/>
     <tableColumn id="2" name="Error type"/>
@@ -847,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,6 +1425,28 @@
         <v>91</v>
       </c>
     </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1418,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,6 +1556,14 @@
       </c>
       <c r="B11" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>